<commit_message>
Completed problem/solution diagram with completed problem argument.
</commit_message>
<xml_diff>
--- a/doc/assurance/ZoneAlertService/3-Requirements/requirements.xlsx
+++ b/doc/assurance/ZoneAlertService/3-Requirements/requirements.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dependable/Contracts/ASTRA/Deliverables/OpenUxAS-ZoneAlert/doc/assurance/ZoneWarningService/3-Requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dependable/Contracts/ASTRA/Deliverables/OpenUxAS-ZoneAlert/doc/assurance/ZoneAlertService/3-Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6936383F-2DFD-7444-B85A-F792D65720C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D1F5A1-6565-8C41-9E32-37E112B5AD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="780" windowWidth="30580" windowHeight="19500" xr2:uid="{A76FD67C-FD1A-274E-A8A0-8B595CED0661}"/>
+    <workbookView xWindow="5260" yWindow="780" windowWidth="30580" windowHeight="19500" activeTab="2" xr2:uid="{A76FD67C-FD1A-274E-A8A0-8B595CED0661}"/>
   </bookViews>
   <sheets>
-    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="Requiremnts Unknowns" sheetId="2" r:id="rId2"/>
+    <sheet name="SoftwareRequirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Interface Def and Reqs" sheetId="3" r:id="rId2"/>
+    <sheet name="Requiremnts Unknowns" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -351,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
@@ -371,7 +372,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -391,9 +391,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -431,7 +431,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -537,7 +537,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -679,7 +679,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -689,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E717DA4B-5271-1F48-AA72-ACE0E1514F9D}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -799,7 +799,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -813,7 +813,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -956,10 +956,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3702B00E-AAB7-7F4B-9F1C-57A3CF73FDCB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA87E05-7BE7-9C44-A27E-E2FA4156C15F}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>